<commit_message>
12/16 adding changes to models for optimization working on thermal optima model
</commit_message>
<xml_diff>
--- a/Temp_dependent_gamma_values_between_host_model.xlsx
+++ b/Temp_dependent_gamma_values_between_host_model.xlsx
@@ -359,7 +359,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.09089872727273</v>
+        <v>0.333330166666667</v>
       </c>
       <c r="B2" t="n">
         <v>24</v>
@@ -367,7 +367,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.1999886</v>
+        <v>0.333330166666667</v>
       </c>
       <c r="B3" t="n">
         <v>26</v>
@@ -375,7 +375,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.33332066666666</v>
+        <v>0.333330166666667</v>
       </c>
       <c r="B4" t="n">
         <v>28</v>
@@ -383,7 +383,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.49998575</v>
+        <v>0.333330166666667</v>
       </c>
       <c r="B5" t="n">
         <v>30</v>
@@ -391,7 +391,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1.71426942857142</v>
+        <v>1.49998575</v>
       </c>
       <c r="B6" t="n">
         <v>32</v>

</xml_diff>